<commit_message>
Cleanup the merged df
</commit_message>
<xml_diff>
--- a/dedup_nessus.xlsx
+++ b/dedup_nessus.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V170"/>
+  <dimension ref="A1:W170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,11 @@
           <t>CANVAS</t>
         </is>
       </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>scanner</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -610,6 +615,7 @@
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -653,7 +659,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>If you do not wish to display this information, edit 'httpd.conf' and
+          <t>NESSUS: If you do not wish to display this information, edit 'httpd.conf' and
 set the directive 'ServerTokens Prod' and restart Apache.</t>
         </is>
       </c>
@@ -678,6 +684,7 @@
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -753,6 +760,7 @@
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -809,7 +817,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Update the AJP configuration to require authorization and/or upgrade the Tomcat server to 7.0.100, 8.5.51, 9.0.31 or later.</t>
+          <t>NESSUS: Update the AJP configuration to require authorization and/or upgrade the Tomcat server to 7.0.100, 8.5.51, 9.0.31 or later.</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -888,6 +896,7 @@
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -944,7 +953,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Update the AJP configuration to require authorization and/or upgrade the Tomcat server to 7.0.100, 8.5.51, 9.0.31 or later.</t>
+          <t>NESSUS: Update the AJP configuration to require authorization and/or upgrade the Tomcat server to 7.0.100, 8.5.51, 9.0.31 or later.</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -1023,6 +1032,7 @@
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1091,6 +1101,7 @@
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1159,6 +1170,7 @@
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1208,7 +1220,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Verify if the remote host has been compromised, and reinstall the
+          <t>NESSUS: Verify if the remote host has been compromised, and reinstall the
 system if necessary.</t>
         </is>
       </c>
@@ -1238,6 +1250,7 @@
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1320,6 +1333,7 @@
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1378,7 +1392,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Consider all cryptographic material generated on the remote host
+          <t>NESSUS: Consider all cryptographic material generated on the remote host
 to be guessable. In particuliar, all SSH, SSL and OpenVPN key
 material should be re-generated.</t>
         </is>
@@ -1410,6 +1424,7 @@
         <v>1</v>
       </c>
       <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1468,7 +1483,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Consider all cryptographic material generated on the remote host to be
+          <t>NESSUS: Consider all cryptographic material generated on the remote host to be
 guessable.  In particuliar, all SSH, SSL and OpenVPN key material should
 be re-generated.</t>
         </is>
@@ -1500,6 +1515,7 @@
         <v>1</v>
       </c>
       <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1558,7 +1574,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Consider all cryptographic material generated on the remote host to be
+          <t>NESSUS: Consider all cryptographic material generated on the remote host to be
 guessable.  In particuliar, all SSH, SSL and OpenVPN key material should
 be re-generated.</t>
         </is>
@@ -1590,6 +1606,7 @@
         <v>1</v>
       </c>
       <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1652,6 +1669,7 @@
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1697,7 +1715,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>It is possible to hide the version number of BIND by using the
+          <t>NESSUS: It is possible to hide the version number of BIND by using the
 'version' directive in the 'options' section in named.conf.</t>
         </is>
       </c>
@@ -1725,6 +1743,7 @@
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1767,7 +1786,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Disable this service if it is not needed or restrict access to
+          <t>NESSUS: Disable this service if it is not needed or restrict access to
 internal hosts only if the service is available externally.</t>
         </is>
       </c>
@@ -1789,6 +1808,7 @@
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1831,7 +1851,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>It may be possible to disable this feature.  Consult the vendor's
+          <t>NESSUS: It may be possible to disable this feature.  Consult the vendor's
 documentation for more information.</t>
         </is>
       </c>
@@ -1856,6 +1876,7 @@
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1923,6 +1944,7 @@
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1987,6 +2009,7 @@
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -2053,6 +2076,7 @@
       <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -2117,6 +2141,7 @@
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -2170,7 +2195,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Disable these HTTP methods. Refer to the plugin output for more information.</t>
+          <t>NESSUS: Disable these HTTP methods. Refer to the plugin output for more information.</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -2237,6 +2262,7 @@
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -2290,7 +2316,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Disable these HTTP methods. Refer to the plugin output for more information.</t>
+          <t>NESSUS: Disable these HTTP methods. Refer to the plugin output for more information.</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -2357,6 +2383,7 @@
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2410,7 +2437,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Disable these HTTP methods. Refer to the plugin output for more information.</t>
+          <t>NESSUS: Disable these HTTP methods. Refer to the plugin output for more information.</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
@@ -2477,6 +2504,7 @@
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr"/>
       <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2576,6 +2604,7 @@
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
       <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2633,7 +2662,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Filter out the ICMP timestamp requests (13), and the outgoing ICMP
+          <t>NESSUS: Filter out the ICMP timestamp requests (13), and the outgoing ICMP
 timestamp replies (14).</t>
         </is>
       </c>
@@ -2660,6 +2689,7 @@
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2719,6 +2749,7 @@
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2776,7 +2807,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Upgrade to BIND 9.11.22, 9.16.6, 9.17.4 or later.</t>
+          <t>NESSUS: Upgrade to BIND 9.11.22, 9.16.6, 9.17.4 or later.</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -2808,6 +2839,7 @@
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
       <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2863,7 +2895,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Upgrade to the patched release most closely related to your current version of BIND.</t>
+          <t>NESSUS: Upgrade to the patched release most closely related to your current version of BIND.</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
@@ -2895,6 +2927,7 @@
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr"/>
       <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2950,7 +2983,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Upgrade to the ISC BIND version referenced in the vendor advisory.</t>
+          <t>NESSUS: Upgrade to the ISC BIND version referenced in the vendor advisory.</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
@@ -2982,6 +3015,7 @@
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
       <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -3045,6 +3079,7 @@
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr"/>
       <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -3110,6 +3145,7 @@
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
       <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -3172,6 +3208,7 @@
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
       <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -3234,6 +3271,7 @@
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr"/>
       <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -3298,6 +3336,7 @@
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr"/>
       <c r="V35" t="inlineStr"/>
+      <c r="W35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -3369,6 +3408,7 @@
       <c r="T36" t="inlineStr"/>
       <c r="U36" t="inlineStr"/>
       <c r="V36" t="inlineStr"/>
+      <c r="W36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -3478,6 +3518,7 @@
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="inlineStr"/>
       <c r="V37" t="inlineStr"/>
+      <c r="W37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -3524,7 +3565,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M38" t="inlineStr"/>
@@ -3545,6 +3586,7 @@
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="inlineStr"/>
       <c r="V38" t="inlineStr"/>
+      <c r="W38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -3591,7 +3633,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M39" t="inlineStr"/>
@@ -3612,6 +3654,7 @@
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="inlineStr"/>
       <c r="V39" t="inlineStr"/>
+      <c r="W39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -3658,7 +3701,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M40" t="inlineStr"/>
@@ -3679,6 +3722,7 @@
       <c r="T40" t="inlineStr"/>
       <c r="U40" t="inlineStr"/>
       <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -3725,7 +3769,7 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M41" t="inlineStr"/>
@@ -3746,6 +3790,7 @@
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr"/>
       <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -3792,7 +3837,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M42" t="inlineStr"/>
@@ -3813,6 +3858,7 @@
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr"/>
       <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -3859,7 +3905,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M43" t="inlineStr"/>
@@ -3880,6 +3926,7 @@
       <c r="T43" t="inlineStr"/>
       <c r="U43" t="inlineStr"/>
       <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -3926,7 +3973,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M44" t="inlineStr"/>
@@ -3947,6 +3994,7 @@
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr"/>
       <c r="V44" t="inlineStr"/>
+      <c r="W44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -3993,7 +4041,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M45" t="inlineStr"/>
@@ -4014,6 +4062,7 @@
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr"/>
       <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -4060,7 +4109,7 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M46" t="inlineStr"/>
@@ -4081,6 +4130,7 @@
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
       <c r="V46" t="inlineStr"/>
+      <c r="W46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -4127,7 +4177,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M47" t="inlineStr"/>
@@ -4148,6 +4198,7 @@
       <c r="T47" t="inlineStr"/>
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr"/>
+      <c r="W47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -4194,7 +4245,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M48" t="inlineStr"/>
@@ -4215,6 +4266,7 @@
       <c r="T48" t="inlineStr"/>
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="inlineStr"/>
+      <c r="W48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -4261,7 +4313,7 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M49" t="inlineStr"/>
@@ -4282,6 +4334,7 @@
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
       <c r="V49" t="inlineStr"/>
+      <c r="W49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -4328,7 +4381,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M50" t="inlineStr"/>
@@ -4349,6 +4402,7 @@
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
       <c r="V50" t="inlineStr"/>
+      <c r="W50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -4395,7 +4449,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M51" t="inlineStr"/>
@@ -4416,6 +4470,7 @@
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
       <c r="V51" t="inlineStr"/>
+      <c r="W51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -4462,7 +4517,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M52" t="inlineStr"/>
@@ -4483,6 +4538,7 @@
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr"/>
       <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -4529,7 +4585,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M53" t="inlineStr"/>
@@ -4550,6 +4606,7 @@
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr"/>
       <c r="V53" t="inlineStr"/>
+      <c r="W53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -4596,7 +4653,7 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M54" t="inlineStr"/>
@@ -4617,6 +4674,7 @@
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr"/>
       <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -4663,7 +4721,7 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M55" t="inlineStr"/>
@@ -4684,6 +4742,7 @@
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr"/>
       <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -4730,7 +4789,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M56" t="inlineStr"/>
@@ -4751,6 +4810,7 @@
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr"/>
       <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -4797,7 +4857,7 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M57" t="inlineStr"/>
@@ -4818,6 +4878,7 @@
       <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr"/>
       <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -4864,7 +4925,7 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M58" t="inlineStr"/>
@@ -4885,6 +4946,7 @@
       <c r="T58" t="inlineStr"/>
       <c r="U58" t="inlineStr"/>
       <c r="V58" t="inlineStr"/>
+      <c r="W58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -4931,7 +4993,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M59" t="inlineStr"/>
@@ -4952,6 +5014,7 @@
       <c r="T59" t="inlineStr"/>
       <c r="U59" t="inlineStr"/>
       <c r="V59" t="inlineStr"/>
+      <c r="W59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -4998,7 +5061,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M60" t="inlineStr"/>
@@ -5019,6 +5082,7 @@
       <c r="T60" t="inlineStr"/>
       <c r="U60" t="inlineStr"/>
       <c r="V60" t="inlineStr"/>
+      <c r="W60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -5065,7 +5129,7 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Protect your target with an IP filter.</t>
+          <t>NESSUS: Protect your target with an IP filter.</t>
         </is>
       </c>
       <c r="M61" t="inlineStr"/>
@@ -5086,6 +5150,7 @@
       <c r="T61" t="inlineStr"/>
       <c r="U61" t="inlineStr"/>
       <c r="V61" t="inlineStr"/>
+      <c r="W61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -5139,7 +5204,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Configure NFS on the remote host so that only authorized hosts can
+          <t>NESSUS: Configure NFS on the remote host so that only authorized hosts can
 mount its remote shares.</t>
         </is>
       </c>
@@ -5192,6 +5257,7 @@
       </c>
       <c r="U62" t="inlineStr"/>
       <c r="V62" t="inlineStr"/>
+      <c r="W62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -5245,7 +5311,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Configure NFS on the remote host so that only authorized hosts can
+          <t>NESSUS: Configure NFS on the remote host so that only authorized hosts can
 mount its remote shares.</t>
         </is>
       </c>
@@ -5298,6 +5364,7 @@
       </c>
       <c r="U63" t="inlineStr"/>
       <c r="V63" t="inlineStr"/>
+      <c r="W63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -5351,7 +5418,7 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Configure NFS on the remote host so that only authorized hosts can
+          <t>NESSUS: Configure NFS on the remote host so that only authorized hosts can
 mount its remote shares.</t>
         </is>
       </c>
@@ -5404,6 +5471,7 @@
       </c>
       <c r="U64" t="inlineStr"/>
       <c r="V64" t="inlineStr"/>
+      <c r="W64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -5445,7 +5513,7 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Ensure each share is intended to be exported.</t>
+          <t>NESSUS: Ensure each share is intended to be exported.</t>
         </is>
       </c>
       <c r="M65" t="inlineStr">
@@ -5473,6 +5541,7 @@
       <c r="T65" t="inlineStr"/>
       <c r="U65" t="inlineStr"/>
       <c r="V65" t="inlineStr"/>
+      <c r="W65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -5521,7 +5590,7 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Place the appropriate restrictions on all NFS shares.</t>
+          <t>NESSUS: Place the appropriate restrictions on all NFS shares.</t>
         </is>
       </c>
       <c r="M66" t="inlineStr">
@@ -5549,6 +5618,7 @@
       <c r="T66" t="inlineStr"/>
       <c r="U66" t="inlineStr"/>
       <c r="V66" t="inlineStr"/>
+      <c r="W66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -5615,6 +5685,7 @@
       <c r="T67" t="inlineStr"/>
       <c r="U67" t="inlineStr"/>
       <c r="V67" t="inlineStr"/>
+      <c r="W67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -5677,6 +5748,7 @@
       <c r="T68" t="inlineStr"/>
       <c r="U68" t="inlineStr"/>
       <c r="V68" t="inlineStr"/>
+      <c r="W68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -5739,6 +5811,7 @@
       <c r="T69" t="inlineStr"/>
       <c r="U69" t="inlineStr"/>
       <c r="V69" t="inlineStr"/>
+      <c r="W69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -5804,6 +5877,7 @@
       <c r="T70" t="inlineStr"/>
       <c r="U70" t="inlineStr"/>
       <c r="V70" t="inlineStr"/>
+      <c r="W70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -5885,6 +5959,7 @@
       <c r="T71" t="inlineStr"/>
       <c r="U71" t="inlineStr"/>
       <c r="V71" t="inlineStr"/>
+      <c r="W71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -5929,7 +6004,7 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Install the patches listed below.</t>
+          <t>NESSUS: Install the patches listed below.</t>
         </is>
       </c>
       <c r="M72" t="inlineStr"/>
@@ -5957,6 +6032,7 @@
       <c r="T72" t="inlineStr"/>
       <c r="U72" t="inlineStr"/>
       <c r="V72" t="inlineStr"/>
+      <c r="W72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -5999,7 +6075,7 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Limit incoming traffic to this port if desired.</t>
+          <t>NESSUS: Limit incoming traffic to this port if desired.</t>
         </is>
       </c>
       <c r="M73" t="inlineStr">
@@ -6020,6 +6096,7 @@
       <c r="T73" t="inlineStr"/>
       <c r="U73" t="inlineStr"/>
       <c r="V73" t="inlineStr"/>
+      <c r="W73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -6130,6 +6207,7 @@
       <c r="T74" t="inlineStr"/>
       <c r="U74" t="inlineStr"/>
       <c r="V74" t="inlineStr"/>
+      <c r="W74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -6200,6 +6278,7 @@
       <c r="T75" t="inlineStr"/>
       <c r="U75" t="inlineStr"/>
       <c r="V75" t="inlineStr"/>
+      <c r="W75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -6257,6 +6336,7 @@
       <c r="T76" t="inlineStr"/>
       <c r="U76" t="inlineStr"/>
       <c r="V76" t="inlineStr"/>
+      <c r="W76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -6320,6 +6400,7 @@
       <c r="T77" t="inlineStr"/>
       <c r="U77" t="inlineStr"/>
       <c r="V77" t="inlineStr"/>
+      <c r="W77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -6384,6 +6465,7 @@
       <c r="T78" t="inlineStr"/>
       <c r="U78" t="inlineStr"/>
       <c r="V78" t="inlineStr"/>
+      <c r="W78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -6450,6 +6532,7 @@
       <c r="T79" t="inlineStr"/>
       <c r="U79" t="inlineStr"/>
       <c r="V79" t="inlineStr"/>
+      <c r="W79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -6516,6 +6599,7 @@
       <c r="T80" t="inlineStr"/>
       <c r="U80" t="inlineStr"/>
       <c r="V80" t="inlineStr"/>
+      <c r="W80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -6582,6 +6666,7 @@
       <c r="T81" t="inlineStr"/>
       <c r="U81" t="inlineStr"/>
       <c r="V81" t="inlineStr"/>
+      <c r="W81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -6646,6 +6731,7 @@
       <c r="T82" t="inlineStr"/>
       <c r="U82" t="inlineStr"/>
       <c r="V82" t="inlineStr"/>
+      <c r="W82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -6712,6 +6798,7 @@
       <c r="T83" t="inlineStr"/>
       <c r="U83" t="inlineStr"/>
       <c r="V83" t="inlineStr"/>
+      <c r="W83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -6778,6 +6865,7 @@
       <c r="T84" t="inlineStr"/>
       <c r="U84" t="inlineStr"/>
       <c r="V84" t="inlineStr"/>
+      <c r="W84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -6842,6 +6930,7 @@
       <c r="T85" t="inlineStr"/>
       <c r="U85" t="inlineStr"/>
       <c r="V85" t="inlineStr"/>
+      <c r="W85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -6905,7 +6994,7 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Upgrade to Samba version 4.2.11 / 4.3.8 / 4.4.2 or later.</t>
+          <t>NESSUS: Upgrade to Samba version 4.2.11 / 4.3.8 / 4.4.2 or later.</t>
         </is>
       </c>
       <c r="M86" t="inlineStr">
@@ -6939,6 +7028,7 @@
       <c r="T86" t="inlineStr"/>
       <c r="U86" t="inlineStr"/>
       <c r="V86" t="inlineStr"/>
+      <c r="W86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -6998,6 +7088,7 @@
       <c r="T87" t="inlineStr"/>
       <c r="U87" t="inlineStr"/>
       <c r="V87" t="inlineStr"/>
+      <c r="W87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -7060,6 +7151,7 @@
       <c r="T88" t="inlineStr"/>
       <c r="U88" t="inlineStr"/>
       <c r="V88" t="inlineStr"/>
+      <c r="W88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -7108,7 +7200,7 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>Disable SMBv1 according to the vendor instructions in Microsoft
+          <t>NESSUS: Disable SMBv1 according to the vendor instructions in Microsoft
 KB2696547. Additionally, block SMB directly by blocking TCP port 445
 on all network boundary devices. For SMB over the NetBIOS API, block
 TCP ports 137 / 139 and UDP ports 137 / 138 on all network boundary
@@ -7147,6 +7239,7 @@
       <c r="T89" t="inlineStr"/>
       <c r="U89" t="inlineStr"/>
       <c r="V89" t="inlineStr"/>
+      <c r="W89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -7207,6 +7300,7 @@
       <c r="T90" t="inlineStr"/>
       <c r="U90" t="inlineStr"/>
       <c r="V90" t="inlineStr"/>
+      <c r="W90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -7267,6 +7361,7 @@
       <c r="T91" t="inlineStr"/>
       <c r="U91" t="inlineStr"/>
       <c r="V91" t="inlineStr"/>
+      <c r="W91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -7327,6 +7422,7 @@
       <c r="T92" t="inlineStr"/>
       <c r="U92" t="inlineStr"/>
       <c r="V92" t="inlineStr"/>
+      <c r="W92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -7387,6 +7483,7 @@
       <c r="T93" t="inlineStr"/>
       <c r="U93" t="inlineStr"/>
       <c r="V93" t="inlineStr"/>
+      <c r="W93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -7447,6 +7544,7 @@
       <c r="T94" t="inlineStr"/>
       <c r="U94" t="inlineStr"/>
       <c r="V94" t="inlineStr"/>
+      <c r="W94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -7507,6 +7605,7 @@
       <c r="T95" t="inlineStr"/>
       <c r="U95" t="inlineStr"/>
       <c r="V95" t="inlineStr"/>
+      <c r="W95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -7571,6 +7670,7 @@
       <c r="T96" t="inlineStr"/>
       <c r="U96" t="inlineStr"/>
       <c r="V96" t="inlineStr"/>
+      <c r="W96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -7620,7 +7720,7 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>Enforce message signing in the host's configuration. On Windows, this
+          <t>NESSUS: Enforce message signing in the host's configuration. On Windows, this
 is found in the policy setting 'Microsoft network server: Digitally
 sign communications (always)'. On Samba, the setting is called 'server
 signing'. See the 'see also' links for further details.</t>
@@ -7648,6 +7748,7 @@
       <c r="T97" t="inlineStr"/>
       <c r="U97" t="inlineStr"/>
       <c r="V97" t="inlineStr"/>
+      <c r="W97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -7691,7 +7792,7 @@
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>Disable this service if you do not use it, or filter incoming traffic
+          <t>NESSUS: Disable this service if you do not use it, or filter incoming traffic
 to this port.</t>
         </is>
       </c>
@@ -7720,6 +7821,7 @@
       <c r="T98" t="inlineStr"/>
       <c r="U98" t="inlineStr"/>
       <c r="V98" t="inlineStr"/>
+      <c r="W98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -7829,6 +7931,7 @@
       <c r="T99" t="inlineStr"/>
       <c r="U99" t="inlineStr"/>
       <c r="V99" t="inlineStr"/>
+      <c r="W99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -7887,7 +7990,7 @@
       </c>
       <c r="L100" t="inlineStr">
         <is>
-          <t>Contact the vendor to see if an update is available.</t>
+          <t>NESSUS: Contact the vendor to see if an update is available.</t>
         </is>
       </c>
       <c r="M100" t="inlineStr">
@@ -7925,6 +8028,7 @@
       <c r="T100" t="inlineStr"/>
       <c r="U100" t="inlineStr"/>
       <c r="V100" t="inlineStr"/>
+      <c r="W100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -7983,7 +8087,7 @@
       </c>
       <c r="L101" t="inlineStr">
         <is>
-          <t>Contact the vendor to see if an update is available.</t>
+          <t>NESSUS: Contact the vendor to see if an update is available.</t>
         </is>
       </c>
       <c r="M101" t="inlineStr">
@@ -8021,6 +8125,7 @@
       <c r="T101" t="inlineStr"/>
       <c r="U101" t="inlineStr"/>
       <c r="V101" t="inlineStr"/>
+      <c r="W101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -8079,7 +8184,7 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>Contact the vendor to see if an update is available.</t>
+          <t>NESSUS: Contact the vendor to see if an update is available.</t>
         </is>
       </c>
       <c r="M102" t="inlineStr">
@@ -8117,6 +8222,7 @@
       <c r="T102" t="inlineStr"/>
       <c r="U102" t="inlineStr"/>
       <c r="V102" t="inlineStr"/>
+      <c r="W102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -8175,7 +8281,7 @@
       </c>
       <c r="L103" t="inlineStr">
         <is>
-          <t>Contact the vendor to see if an update is available.</t>
+          <t>NESSUS: Contact the vendor to see if an update is available.</t>
         </is>
       </c>
       <c r="M103" t="inlineStr">
@@ -8213,6 +8319,7 @@
       <c r="T103" t="inlineStr"/>
       <c r="U103" t="inlineStr"/>
       <c r="V103" t="inlineStr"/>
+      <c r="W103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -8271,7 +8378,7 @@
       </c>
       <c r="L104" t="inlineStr">
         <is>
-          <t>Contact the vendor to see if an update is available.</t>
+          <t>NESSUS: Contact the vendor to see if an update is available.</t>
         </is>
       </c>
       <c r="M104" t="inlineStr">
@@ -8309,6 +8416,7 @@
       <c r="T104" t="inlineStr"/>
       <c r="U104" t="inlineStr"/>
       <c r="V104" t="inlineStr"/>
+      <c r="W104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -8367,7 +8475,7 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>Contact the vendor to see if an update is available.</t>
+          <t>NESSUS: Contact the vendor to see if an update is available.</t>
         </is>
       </c>
       <c r="M105" t="inlineStr">
@@ -8405,6 +8513,7 @@
       <c r="T105" t="inlineStr"/>
       <c r="U105" t="inlineStr"/>
       <c r="V105" t="inlineStr"/>
+      <c r="W105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -8524,6 +8633,7 @@
       <c r="T106" t="inlineStr"/>
       <c r="U106" t="inlineStr"/>
       <c r="V106" t="inlineStr"/>
+      <c r="W106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -8582,6 +8692,7 @@
       <c r="T107" t="inlineStr"/>
       <c r="U107" t="inlineStr"/>
       <c r="V107" t="inlineStr"/>
+      <c r="W107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -8645,6 +8756,7 @@
       <c r="T108" t="inlineStr"/>
       <c r="U108" t="inlineStr"/>
       <c r="V108" t="inlineStr"/>
+      <c r="W108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -8700,7 +8812,7 @@
       </c>
       <c r="L109" t="inlineStr">
         <is>
-          <t>Contact the vendor or consult product documentation to disable CBC mode
+          <t>NESSUS: Contact the vendor or consult product documentation to disable CBC mode
 cipher encryption, and enable CTR or GCM cipher mode encryption.</t>
         </is>
       </c>
@@ -8747,6 +8859,7 @@
       <c r="T109" t="inlineStr"/>
       <c r="U109" t="inlineStr"/>
       <c r="V109" t="inlineStr"/>
+      <c r="W109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -8813,6 +8926,7 @@
       <c r="T110" t="inlineStr"/>
       <c r="U110" t="inlineStr"/>
       <c r="V110" t="inlineStr"/>
+      <c r="W110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -8881,6 +8995,7 @@
       <c r="T111" t="inlineStr"/>
       <c r="U111" t="inlineStr"/>
       <c r="V111" t="inlineStr"/>
+      <c r="W111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -8931,7 +9046,7 @@
       </c>
       <c r="L112" t="inlineStr">
         <is>
-          <t>Contact the vendor or consult product documentation to remove the weak
+          <t>NESSUS: Contact the vendor or consult product documentation to remove the weak
 ciphers.</t>
         </is>
       </c>
@@ -8966,6 +9081,7 @@
       <c r="T112" t="inlineStr"/>
       <c r="U112" t="inlineStr"/>
       <c r="V112" t="inlineStr"/>
+      <c r="W112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -9024,7 +9140,7 @@
       </c>
       <c r="L113" t="inlineStr">
         <is>
-          <t>Contact the vendor or consult product documentation to disable the weak algorithms.</t>
+          <t>NESSUS: Contact the vendor or consult product documentation to disable the weak algorithms.</t>
         </is>
       </c>
       <c r="M113" t="inlineStr">
@@ -9053,6 +9169,7 @@
       <c r="T113" t="inlineStr"/>
       <c r="U113" t="inlineStr"/>
       <c r="V113" t="inlineStr"/>
+      <c r="W113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -9104,7 +9221,7 @@
       </c>
       <c r="L114" t="inlineStr">
         <is>
-          <t>Contact the vendor or consult product documentation to disable MD5 and
+          <t>NESSUS: Contact the vendor or consult product documentation to disable MD5 and
 96-bit MAC algorithms.</t>
         </is>
       </c>
@@ -9137,6 +9254,7 @@
       <c r="T114" t="inlineStr"/>
       <c r="U114" t="inlineStr"/>
       <c r="V114" t="inlineStr"/>
+      <c r="W114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -9198,6 +9316,7 @@
       <c r="T115" t="inlineStr"/>
       <c r="U115" t="inlineStr"/>
       <c r="V115" t="inlineStr"/>
+      <c r="W115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -9259,6 +9378,7 @@
       <c r="T116" t="inlineStr"/>
       <c r="U116" t="inlineStr"/>
       <c r="V116" t="inlineStr"/>
+      <c r="W116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -9316,7 +9436,7 @@
       </c>
       <c r="L117" t="inlineStr">
         <is>
-          <t>Reconfigure the affected application if possible to avoid use of weak
+          <t>NESSUS: Reconfigure the affected application if possible to avoid use of weak
 ciphers.</t>
         </is>
       </c>
@@ -9370,6 +9490,7 @@
       <c r="T117" t="inlineStr"/>
       <c r="U117" t="inlineStr"/>
       <c r="V117" t="inlineStr"/>
+      <c r="W117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -9414,7 +9535,7 @@
       </c>
       <c r="L118" t="inlineStr">
         <is>
-          <t>If the machine has several names, make sure that users connect to the
+          <t>NESSUS: If the machine has several names, make sure that users connect to the
 service through the DNS hostname that matches the common name in the
 certificate.</t>
         </is>
@@ -9442,6 +9563,7 @@
       <c r="T118" t="inlineStr"/>
       <c r="U118" t="inlineStr"/>
       <c r="V118" t="inlineStr"/>
+      <c r="W118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -9486,7 +9608,7 @@
       </c>
       <c r="L119" t="inlineStr">
         <is>
-          <t>If the machine has several names, make sure that users connect to the
+          <t>NESSUS: If the machine has several names, make sure that users connect to the
 service through the DNS hostname that matches the common name in the
 certificate.</t>
         </is>
@@ -9514,6 +9636,7 @@
       <c r="T119" t="inlineStr"/>
       <c r="U119" t="inlineStr"/>
       <c r="V119" t="inlineStr"/>
+      <c r="W119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -9587,7 +9710,7 @@
       </c>
       <c r="L120" t="inlineStr">
         <is>
-          <t>Purchase or generate a proper SSL certificate for this service.</t>
+          <t>NESSUS: Purchase or generate a proper SSL certificate for this service.</t>
         </is>
       </c>
       <c r="M120" t="inlineStr">
@@ -9623,6 +9746,7 @@
       <c r="T120" t="inlineStr"/>
       <c r="U120" t="inlineStr"/>
       <c r="V120" t="inlineStr"/>
+      <c r="W120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -9696,7 +9820,7 @@
       </c>
       <c r="L121" t="inlineStr">
         <is>
-          <t>Purchase or generate a proper SSL certificate for this service.</t>
+          <t>NESSUS: Purchase or generate a proper SSL certificate for this service.</t>
         </is>
       </c>
       <c r="M121" t="inlineStr">
@@ -9732,6 +9856,7 @@
       <c r="T121" t="inlineStr"/>
       <c r="U121" t="inlineStr"/>
       <c r="V121" t="inlineStr"/>
+      <c r="W121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -9781,7 +9906,7 @@
       </c>
       <c r="L122" t="inlineStr">
         <is>
-          <t>Purchase or generate a new SSL certificate to replace the existing
+          <t>NESSUS: Purchase or generate a new SSL certificate to replace the existing
 one.</t>
         </is>
       </c>
@@ -9809,6 +9934,7 @@
       <c r="T122" t="inlineStr"/>
       <c r="U122" t="inlineStr"/>
       <c r="V122" t="inlineStr"/>
+      <c r="W122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -9858,7 +9984,7 @@
       </c>
       <c r="L123" t="inlineStr">
         <is>
-          <t>Purchase or generate a new SSL certificate to replace the existing
+          <t>NESSUS: Purchase or generate a new SSL certificate to replace the existing
 one.</t>
         </is>
       </c>
@@ -9886,6 +10012,7 @@
       <c r="T123" t="inlineStr"/>
       <c r="U123" t="inlineStr"/>
       <c r="V123" t="inlineStr"/>
+      <c r="W123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -9993,6 +10120,7 @@
       <c r="T124" t="inlineStr"/>
       <c r="U124" t="inlineStr"/>
       <c r="V124" t="inlineStr"/>
+      <c r="W124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -10100,6 +10228,7 @@
       <c r="T125" t="inlineStr"/>
       <c r="U125" t="inlineStr"/>
       <c r="V125" t="inlineStr"/>
+      <c r="W125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -10148,7 +10277,7 @@
       </c>
       <c r="L126" t="inlineStr">
         <is>
-          <t>Purchase or generate a proper SSL certificate for this service.</t>
+          <t>NESSUS: Purchase or generate a proper SSL certificate for this service.</t>
         </is>
       </c>
       <c r="M126" t="inlineStr"/>
@@ -10175,6 +10304,7 @@
       <c r="T126" t="inlineStr"/>
       <c r="U126" t="inlineStr"/>
       <c r="V126" t="inlineStr"/>
+      <c r="W126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -10223,7 +10353,7 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>Purchase or generate a proper SSL certificate for this service.</t>
+          <t>NESSUS: Purchase or generate a proper SSL certificate for this service.</t>
         </is>
       </c>
       <c r="M127" t="inlineStr"/>
@@ -10250,6 +10380,7 @@
       <c r="T127" t="inlineStr"/>
       <c r="U127" t="inlineStr"/>
       <c r="V127" t="inlineStr"/>
+      <c r="W127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -10355,6 +10486,7 @@
       <c r="T128" t="inlineStr"/>
       <c r="U128" t="inlineStr"/>
       <c r="V128" t="inlineStr"/>
+      <c r="W128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -10445,6 +10577,7 @@
       <c r="T129" t="inlineStr"/>
       <c r="U129" t="inlineStr"/>
       <c r="V129" t="inlineStr"/>
+      <c r="W129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -10598,6 +10731,7 @@
       <c r="T130" t="inlineStr"/>
       <c r="U130" t="inlineStr"/>
       <c r="V130" t="inlineStr"/>
+      <c r="W130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -10703,6 +10837,7 @@
       <c r="T131" t="inlineStr"/>
       <c r="U131" t="inlineStr"/>
       <c r="V131" t="inlineStr"/>
+      <c r="W131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -10774,6 +10909,7 @@
       <c r="T132" t="inlineStr"/>
       <c r="U132" t="inlineStr"/>
       <c r="V132" t="inlineStr"/>
+      <c r="W132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -10845,6 +10981,7 @@
       <c r="T133" t="inlineStr"/>
       <c r="U133" t="inlineStr"/>
       <c r="V133" t="inlineStr"/>
+      <c r="W133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -10906,7 +11043,7 @@
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>Disable SSLv2 and export grade cryptography cipher suites. Ensure that
+          <t>NESSUS: Disable SSLv2 and export grade cryptography cipher suites. Ensure that
 private keys are not used anywhere with server software that supports
 SSLv2 connections.</t>
         </is>
@@ -10960,6 +11097,7 @@
       <c r="T134" t="inlineStr"/>
       <c r="U134" t="inlineStr"/>
       <c r="V134" t="inlineStr"/>
+      <c r="W134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -11016,7 +11154,7 @@
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>Reconfigure the affected application if possible to avoid use of
+          <t>NESSUS: Reconfigure the affected application if possible to avoid use of
 medium strength ciphers.</t>
         </is>
       </c>
@@ -11059,6 +11197,7 @@
       <c r="T135" t="inlineStr"/>
       <c r="U135" t="inlineStr"/>
       <c r="V135" t="inlineStr"/>
+      <c r="W135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -11115,7 +11254,7 @@
       </c>
       <c r="L136" t="inlineStr">
         <is>
-          <t>Reconfigure the affected application if possible to avoid use of
+          <t>NESSUS: Reconfigure the affected application if possible to avoid use of
 medium strength ciphers.</t>
         </is>
       </c>
@@ -11156,6 +11295,7 @@
       <c r="T136" t="inlineStr"/>
       <c r="U136" t="inlineStr"/>
       <c r="V136" t="inlineStr"/>
+      <c r="W136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -11248,6 +11388,7 @@
       <c r="T137" t="inlineStr"/>
       <c r="U137" t="inlineStr"/>
       <c r="V137" t="inlineStr"/>
+      <c r="W137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -11335,6 +11476,7 @@
       <c r="T138" t="inlineStr"/>
       <c r="U138" t="inlineStr"/>
       <c r="V138" t="inlineStr"/>
+      <c r="W138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -11392,7 +11534,7 @@
       </c>
       <c r="L139" t="inlineStr">
         <is>
-          <t>Reconfigure the affected application, if possible, to avoid use of RC4
+          <t>NESSUS: Reconfigure the affected application, if possible, to avoid use of RC4
 ciphers. Consider using TLS 1.2 with AES-GCM suites subject to browser
 and web server support.</t>
         </is>
@@ -11450,6 +11592,7 @@
       <c r="T139" t="inlineStr"/>
       <c r="U139" t="inlineStr"/>
       <c r="V139" t="inlineStr"/>
+      <c r="W139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -11507,7 +11650,7 @@
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>Reconfigure the affected application, if possible, to avoid use of RC4
+          <t>NESSUS: Reconfigure the affected application, if possible, to avoid use of RC4
 ciphers. Consider using TLS 1.2 with AES-GCM suites subject to browser
 and web server support.</t>
         </is>
@@ -11565,6 +11708,7 @@
       <c r="T140" t="inlineStr"/>
       <c r="U140" t="inlineStr"/>
       <c r="V140" t="inlineStr"/>
+      <c r="W140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -11622,7 +11766,7 @@
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>Reconfigure the affected application, if possible, to avoid use of RC4
+          <t>NESSUS: Reconfigure the affected application, if possible, to avoid use of RC4
 ciphers. Consider using TLS 1.2 with AES-GCM suites subject to browser
 and web server support.</t>
         </is>
@@ -11671,6 +11815,7 @@
       <c r="T141" t="inlineStr"/>
       <c r="U141" t="inlineStr"/>
       <c r="V141" t="inlineStr"/>
+      <c r="W141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -11728,7 +11873,7 @@
       </c>
       <c r="L142" t="inlineStr">
         <is>
-          <t>Reconfigure the affected application, if possible, to avoid use of RC4
+          <t>NESSUS: Reconfigure the affected application, if possible, to avoid use of RC4
 ciphers. Consider using TLS 1.2 with AES-GCM suites subject to browser
 and web server support.</t>
         </is>
@@ -11777,6 +11922,7 @@
       <c r="T142" t="inlineStr"/>
       <c r="U142" t="inlineStr"/>
       <c r="V142" t="inlineStr"/>
+      <c r="W142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -11831,7 +11977,7 @@
       </c>
       <c r="L143" t="inlineStr">
         <is>
-          <t>Purchase or generate a proper SSL certificate for this service.</t>
+          <t>NESSUS: Purchase or generate a proper SSL certificate for this service.</t>
         </is>
       </c>
       <c r="M143" t="inlineStr"/>
@@ -11857,6 +12003,7 @@
       <c r="T143" t="inlineStr"/>
       <c r="U143" t="inlineStr"/>
       <c r="V143" t="inlineStr"/>
+      <c r="W143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -11911,7 +12058,7 @@
       </c>
       <c r="L144" t="inlineStr">
         <is>
-          <t>Purchase or generate a proper SSL certificate for this service.</t>
+          <t>NESSUS: Purchase or generate a proper SSL certificate for this service.</t>
         </is>
       </c>
       <c r="M144" t="inlineStr"/>
@@ -11937,6 +12084,7 @@
       <c r="T144" t="inlineStr"/>
       <c r="U144" t="inlineStr"/>
       <c r="V144" t="inlineStr"/>
+      <c r="W144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -12001,6 +12149,7 @@
       <c r="T145" t="inlineStr"/>
       <c r="U145" t="inlineStr"/>
       <c r="V145" t="inlineStr"/>
+      <c r="W145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -12066,7 +12215,7 @@
       </c>
       <c r="L146" t="inlineStr">
         <is>
-          <t>Consult the application's documentation to disable SSL 2.0 and 3.0.
+          <t>NESSUS: Consult the application's documentation to disable SSL 2.0 and 3.0.
 Use TLS 1.2 (with approved cipher suites) or higher instead.</t>
         </is>
       </c>
@@ -12162,6 +12311,7 @@
       <c r="T146" t="inlineStr"/>
       <c r="U146" t="inlineStr"/>
       <c r="V146" t="inlineStr"/>
+      <c r="W146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -12227,7 +12377,7 @@
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>Consult the application's documentation to disable SSL 2.0 and 3.0.
+          <t>NESSUS: Consult the application's documentation to disable SSL 2.0 and 3.0.
 Use TLS 1.2 (with approved cipher suites) or higher instead.</t>
         </is>
       </c>
@@ -12284,6 +12434,7 @@
       <c r="T147" t="inlineStr"/>
       <c r="U147" t="inlineStr"/>
       <c r="V147" t="inlineStr"/>
+      <c r="W147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -12334,7 +12485,7 @@
       </c>
       <c r="L148" t="inlineStr">
         <is>
-          <t>Reconfigure the affected application, if possible to avoid the use of
+          <t>NESSUS: Reconfigure the affected application, if possible to avoid the use of
 weak ciphers.</t>
         </is>
       </c>
@@ -12388,6 +12539,7 @@
       <c r="T148" t="inlineStr"/>
       <c r="U148" t="inlineStr"/>
       <c r="V148" t="inlineStr"/>
+      <c r="W148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -12444,7 +12596,7 @@
       </c>
       <c r="L149" t="inlineStr">
         <is>
-          <t>Reconfigure the service to remove support for EXPORT_DHE cipher
+          <t>NESSUS: Reconfigure the service to remove support for EXPORT_DHE cipher
 suites.</t>
         </is>
       </c>
@@ -12492,6 +12644,7 @@
       <c r="T149" t="inlineStr"/>
       <c r="U149" t="inlineStr"/>
       <c r="V149" t="inlineStr"/>
+      <c r="W149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -12548,7 +12701,7 @@
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>Reconfigure the service to remove support for EXPORT_RSA cipher
+          <t>NESSUS: Reconfigure the service to remove support for EXPORT_RSA cipher
 suites.</t>
         </is>
       </c>
@@ -12598,6 +12751,7 @@
       <c r="T150" t="inlineStr"/>
       <c r="U150" t="inlineStr"/>
       <c r="V150" t="inlineStr"/>
+      <c r="W150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -12653,7 +12807,7 @@
       </c>
       <c r="L151" t="inlineStr">
         <is>
-          <t>Only enable support for recommened cipher suites.</t>
+          <t>NESSUS: Only enable support for recommened cipher suites.</t>
         </is>
       </c>
       <c r="M151" t="inlineStr">
@@ -12722,6 +12876,7 @@
       <c r="T151" t="inlineStr"/>
       <c r="U151" t="inlineStr"/>
       <c r="V151" t="inlineStr"/>
+      <c r="W151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -12777,7 +12932,7 @@
       </c>
       <c r="L152" t="inlineStr">
         <is>
-          <t>Only enable support for recommened cipher suites.</t>
+          <t>NESSUS: Only enable support for recommened cipher suites.</t>
         </is>
       </c>
       <c r="M152" t="inlineStr">
@@ -12825,6 +12980,7 @@
       <c r="T152" t="inlineStr"/>
       <c r="U152" t="inlineStr"/>
       <c r="V152" t="inlineStr"/>
+      <c r="W152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -12893,7 +13049,7 @@
       </c>
       <c r="L153" t="inlineStr">
         <is>
-          <t>Disable SSLv3.
+          <t>NESSUS: Disable SSLv3.
 Services that must support SSLv3 should enable the TLS Fallback SCSV
 mechanism until SSLv3 can be disabled.</t>
         </is>
@@ -12934,6 +13090,7 @@
       <c r="T153" t="inlineStr"/>
       <c r="U153" t="inlineStr"/>
       <c r="V153" t="inlineStr"/>
+      <c r="W153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -13002,7 +13159,7 @@
       </c>
       <c r="L154" t="inlineStr">
         <is>
-          <t>Disable SSLv3.
+          <t>NESSUS: Disable SSLv3.
 Services that must support SSLv3 should enable the TLS Fallback SCSV
 mechanism until SSLv3 can be disabled.</t>
         </is>
@@ -13043,6 +13200,7 @@
       <c r="T154" t="inlineStr"/>
       <c r="U154" t="inlineStr"/>
       <c r="V154" t="inlineStr"/>
+      <c r="W154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -13132,6 +13290,7 @@
       <c r="T155" t="inlineStr"/>
       <c r="U155" t="inlineStr"/>
       <c r="V155" t="inlineStr"/>
+      <c r="W155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -13192,6 +13351,7 @@
       <c r="T156" t="inlineStr"/>
       <c r="U156" t="inlineStr"/>
       <c r="V156" t="inlineStr"/>
+      <c r="W156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -13235,7 +13395,7 @@
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>Disable this service if you do not use it.</t>
+          <t>NESSUS: Disable this service if you do not use it.</t>
         </is>
       </c>
       <c r="M157" t="inlineStr"/>
@@ -13252,6 +13412,7 @@
       <c r="T157" t="inlineStr"/>
       <c r="U157" t="inlineStr"/>
       <c r="V157" t="inlineStr"/>
+      <c r="W157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -13308,7 +13469,7 @@
       </c>
       <c r="L158" t="inlineStr">
         <is>
-          <t>Enable support for TLS 1.2 and 1.3, and disable support for TLS 1.0.</t>
+          <t>NESSUS: Enable support for TLS 1.2 and 1.3, and disable support for TLS 1.0.</t>
         </is>
       </c>
       <c r="M158" t="inlineStr">
@@ -13337,6 +13498,7 @@
       <c r="T158" t="inlineStr"/>
       <c r="U158" t="inlineStr"/>
       <c r="V158" t="inlineStr"/>
+      <c r="W158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -13393,7 +13555,7 @@
       </c>
       <c r="L159" t="inlineStr">
         <is>
-          <t>Enable support for TLS 1.2 and 1.3, and disable support for TLS 1.0.</t>
+          <t>NESSUS: Enable support for TLS 1.2 and 1.3, and disable support for TLS 1.0.</t>
         </is>
       </c>
       <c r="M159" t="inlineStr">
@@ -13422,6 +13584,7 @@
       <c r="T159" t="inlineStr"/>
       <c r="U159" t="inlineStr"/>
       <c r="V159" t="inlineStr"/>
+      <c r="W159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -13484,6 +13647,7 @@
       <c r="T160" t="inlineStr"/>
       <c r="U160" t="inlineStr"/>
       <c r="V160" t="inlineStr"/>
+      <c r="W160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -13609,6 +13773,7 @@
       <c r="T161" t="inlineStr"/>
       <c r="U161" t="inlineStr"/>
       <c r="V161" t="inlineStr"/>
+      <c r="W161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -13660,7 +13825,7 @@
       </c>
       <c r="L162" t="inlineStr">
         <is>
-          <t>Secure the VNC service with a strong password.</t>
+          <t>NESSUS: Secure the VNC service with a strong password.</t>
         </is>
       </c>
       <c r="M162" t="inlineStr"/>
@@ -13683,6 +13848,7 @@
       <c r="T162" t="inlineStr"/>
       <c r="U162" t="inlineStr"/>
       <c r="V162" t="inlineStr"/>
+      <c r="W162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -13742,6 +13908,7 @@
       <c r="T163" t="inlineStr"/>
       <c r="U163" t="inlineStr"/>
       <c r="V163" t="inlineStr"/>
+      <c r="W163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -13807,6 +13974,7 @@
       <c r="T164" t="inlineStr"/>
       <c r="U164" t="inlineStr"/>
       <c r="V164" t="inlineStr"/>
+      <c r="W164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -13851,7 +14019,7 @@
       </c>
       <c r="L165" t="inlineStr">
         <is>
-          <t>Make sure use of this software is done in accordance with your
+          <t>NESSUS: Make sure use of this software is done in accordance with your
 organization's security policy and filter incoming traffic to this
 port.</t>
         </is>
@@ -13881,6 +14049,7 @@
       <c r="T165" t="inlineStr"/>
       <c r="U165" t="inlineStr"/>
       <c r="V165" t="inlineStr"/>
+      <c r="W165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -13947,6 +14116,7 @@
       <c r="T166" t="inlineStr"/>
       <c r="U166" t="inlineStr"/>
       <c r="V166" t="inlineStr"/>
+      <c r="W166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -13991,7 +14161,7 @@
       </c>
       <c r="L167" t="inlineStr">
         <is>
-          <t>http://support.microsoft.com/default.aspx?kbid=241520</t>
+          <t>NESSUS: http://support.microsoft.com/default.aspx?kbid=241520</t>
         </is>
       </c>
       <c r="M167" t="inlineStr"/>
@@ -14008,6 +14178,7 @@
       <c r="T167" t="inlineStr"/>
       <c r="U167" t="inlineStr"/>
       <c r="V167" t="inlineStr"/>
+      <c r="W167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -14077,6 +14248,7 @@
       <c r="T168" t="inlineStr"/>
       <c r="U168" t="inlineStr"/>
       <c r="V168" t="inlineStr"/>
+      <c r="W168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -14144,6 +14316,7 @@
       <c r="T169" t="inlineStr"/>
       <c r="U169" t="inlineStr"/>
       <c r="V169" t="inlineStr"/>
+      <c r="W169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -14195,7 +14368,7 @@
       </c>
       <c r="L170" t="inlineStr">
         <is>
-          <t>Restrict access to this port. If the X11 client/server facility is not
+          <t>NESSUS: Restrict access to this port. If the X11 client/server facility is not
 used, disable TCP support in X11 entirely (-nolisten tcp).</t>
         </is>
       </c>
@@ -14219,6 +14392,7 @@
       <c r="T170" t="inlineStr"/>
       <c r="U170" t="inlineStr"/>
       <c r="V170" t="inlineStr"/>
+      <c r="W170" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>